<commit_message>
Fix answers and hints and new conda env
</commit_message>
<xml_diff>
--- a/static/files/puns_hints.xlsx
+++ b/static/files/puns_hints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\Documents\GitHub\Puns\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AF3AE0-C597-4F67-9293-6F6BA4F11527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA637708-7AA2-4A27-A011-D1A6AC6957DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22020" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24580" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="puns" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
   <si>
     <t>question</t>
   </si>
@@ -695,6 +695,15 @@
   </si>
   <si>
     <t>How can computers get a hangover</t>
+  </si>
+  <si>
+    <t>What kind of fish you find in a hospital</t>
+  </si>
+  <si>
+    <t>The last specialist you'd want to see in a hospital.</t>
+  </si>
+  <si>
+    <t>A sturgeon.</t>
   </si>
 </sst>
 </file>
@@ -1253,9 +1262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1293,7 +1302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1399,7 +1408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1541,7 +1550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,21 +1558,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="91.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="91.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="141.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="91.109375" style="1"/>
+    <col min="1" max="1" width="141.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="91.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -1585,7 +1594,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
@@ -1607,7 +1616,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>224</v>
       </c>
@@ -1618,18 +1627,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1640,18 +1649,18 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>94</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -1717,7 +1726,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -1750,7 +1759,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>96</v>
       </c>
@@ -1761,7 +1770,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>218</v>
       </c>
@@ -1783,7 +1792,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1794,7 +1803,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>90</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1827,7 +1836,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1838,7 +1847,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -1849,7 +1858,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -1871,7 +1880,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1882,7 +1891,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
@@ -1893,7 +1902,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1904,7 +1913,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1915,7 +1924,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>192</v>
       </c>
@@ -1926,7 +1935,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>120</v>
       </c>
@@ -1948,7 +1957,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1959,7 +1968,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
@@ -1970,7 +1979,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>73</v>
       </c>
@@ -1981,7 +1990,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>122</v>
       </c>
@@ -1992,7 +2001,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>114</v>
       </c>
@@ -2003,7 +2012,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
@@ -2014,7 +2023,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
@@ -2025,7 +2034,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>216</v>
       </c>
@@ -2036,7 +2045,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>116</v>
       </c>
@@ -2047,7 +2056,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>112</v>
       </c>
@@ -2058,7 +2067,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>84</v>
       </c>
@@ -2069,7 +2078,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
@@ -2080,7 +2089,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>124</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -2102,7 +2111,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>223</v>
       </c>
@@ -2113,7 +2122,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>18</v>
       </c>
@@ -2124,7 +2133,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>106</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -2146,7 +2155,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -2157,7 +2166,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>80</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>211</v>
       </c>
@@ -2179,7 +2188,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
@@ -2190,7 +2199,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>102</v>
       </c>
@@ -2201,7 +2210,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>75</v>
       </c>
@@ -2212,7 +2221,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>33</v>
       </c>
@@ -2223,7 +2232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>24</v>
       </c>
@@ -2234,7 +2243,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>86</v>
       </c>
@@ -2245,7 +2254,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
@@ -2256,7 +2265,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>43</v>
       </c>
@@ -2267,7 +2276,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
@@ -2278,7 +2287,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>213</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>29</v>
       </c>
@@ -2300,7 +2309,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>49</v>
       </c>
@@ -2322,7 +2331,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>26</v>
       </c>
@@ -2333,7 +2342,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>104</v>
       </c>
@@ -2344,7 +2353,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>212</v>
       </c>
@@ -2355,7 +2364,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>63</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
@@ -2377,7 +2386,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>217</v>
       </c>
@@ -2388,9 +2397,20 @@
         <v>207</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
-    <sortCondition ref="A2:A75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
+    <sortCondition ref="A2:A74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>